<commit_message>
Change Management plan adding
</commit_message>
<xml_diff>
--- a/Definition/Design/WBS_Dictionary.xlsx
+++ b/Definition/Design/WBS_Dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nadaf\Desktop\ITI\QA\QA workshop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ossay\Downloads\New folder\TravelAdvisor\Definition\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7E357D4-AF35-4993-A52E-265B3694AE68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A12C60C2-FBC8-4631-B0DB-0D5AB1E54F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WBS Dictionary" sheetId="2" r:id="rId1"/>
@@ -313,14 +313,14 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -340,7 +340,7 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -348,7 +348,7 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -388,7 +388,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -407,7 +407,7 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -895,33 +895,33 @@
   <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.875" style="1" customWidth="1"/>
     <col min="3" max="3" width="45" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.36328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.375" style="1" customWidth="1"/>
     <col min="5" max="5" width="24" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" style="1" customWidth="1"/>
-    <col min="7" max="8" width="16.81640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.125" style="1" customWidth="1"/>
+    <col min="7" max="8" width="16.875" style="1" customWidth="1"/>
     <col min="9" max="9" width="36" style="1" customWidth="1"/>
     <col min="10" max="10" width="3" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="10.81640625" style="1"/>
+    <col min="11" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" customFormat="1" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6"/>
       <c r="B1" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D1" s="7"/>
     </row>
-    <row r="2" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="4"/>
       <c r="C2" s="17" t="s">
         <v>0</v>
@@ -938,7 +938,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2"/>
       <c r="C3" s="22" t="s">
         <v>26</v>
@@ -955,10 +955,10 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="4"/>
     </row>
-    <row r="5" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="19" t="s">
         <v>9</v>
       </c>
@@ -984,7 +984,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="8">
         <v>1</v>
       </c>
@@ -1003,7 +1003,7 @@
       <c r="H6" s="11"/>
       <c r="I6" s="9"/>
     </row>
-    <row r="7" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="14">
         <v>1.1000000000000001</v>
       </c>
@@ -1027,7 +1027,7 @@
       </c>
       <c r="I7" s="14"/>
     </row>
-    <row r="8" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>1</v>
       </c>
@@ -1047,7 +1047,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>2</v>
       </c>
@@ -1071,7 +1071,7 @@
       </c>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="14">
         <v>1.2</v>
       </c>
@@ -1095,7 +1095,7 @@
       </c>
       <c r="I10" s="13"/>
     </row>
-    <row r="11" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="8">
         <v>2</v>
       </c>
@@ -1111,7 +1111,7 @@
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
     </row>
-    <row r="12" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="14">
         <v>2.1</v>
       </c>
@@ -1135,7 +1135,7 @@
       </c>
       <c r="I12" s="14"/>
     </row>
-    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="14" t="s">
         <v>3</v>
       </c>
@@ -1159,7 +1159,7 @@
       </c>
       <c r="I13" s="13"/>
     </row>
-    <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="14" t="s">
         <v>4</v>
       </c>
@@ -1185,7 +1185,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="14" t="s">
         <v>37</v>
       </c>
@@ -1209,7 +1209,7 @@
       </c>
       <c r="I15" s="14"/>
     </row>
-    <row r="16" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
         <v>38</v>
       </c>
@@ -1233,7 +1233,7 @@
       </c>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>39</v>
       </c>
@@ -1257,7 +1257,7 @@
       </c>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
         <v>40</v>
       </c>
@@ -1281,7 +1281,7 @@
       </c>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="14" t="s">
         <v>41</v>
       </c>
@@ -1305,7 +1305,7 @@
       </c>
       <c r="I19" s="13"/>
     </row>
-    <row r="20" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="14" t="s">
         <v>42</v>
       </c>
@@ -1329,7 +1329,7 @@
       </c>
       <c r="I20" s="13"/>
     </row>
-    <row r="21" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="14" t="s">
         <v>45</v>
       </c>
@@ -1353,7 +1353,7 @@
       </c>
       <c r="I21" s="14"/>
     </row>
-    <row r="22" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
         <v>46</v>
       </c>
@@ -1377,7 +1377,7 @@
       </c>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="14" t="s">
         <v>47</v>
       </c>
@@ -1401,7 +1401,7 @@
       </c>
       <c r="I23" s="14"/>
     </row>
-    <row r="24" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
         <v>50</v>
       </c>
@@ -1425,7 +1425,7 @@
       </c>
       <c r="I24" s="3"/>
     </row>
-    <row r="25" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="8">
         <v>3</v>
       </c>
@@ -1442,7 +1442,7 @@
       <c r="H25" s="11"/>
       <c r="I25" s="9"/>
     </row>
-    <row r="26" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="13">
         <v>3.1</v>
       </c>
@@ -1462,7 +1462,7 @@
       <c r="H26" s="16"/>
       <c r="I26" s="14"/>
     </row>
-    <row r="27" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="2" t="s">
         <v>5</v>
       </c>
@@ -1482,7 +1482,7 @@
       <c r="H27" s="5"/>
       <c r="I27" s="3"/>
     </row>
-    <row r="28" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="2" t="s">
         <v>64</v>
       </c>
@@ -1502,7 +1502,7 @@
       <c r="H28" s="5"/>
       <c r="I28" s="3"/>
     </row>
-    <row r="29" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="13">
         <v>3.2</v>
       </c>
@@ -1522,7 +1522,7 @@
       <c r="H29" s="16"/>
       <c r="I29" s="14"/>
     </row>
-    <row r="30" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="2" t="s">
         <v>6</v>
       </c>
@@ -1542,7 +1542,7 @@
       <c r="H30" s="5"/>
       <c r="I30" s="3"/>
     </row>
-    <row r="31" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="2" t="s">
         <v>65</v>
       </c>
@@ -1562,7 +1562,7 @@
       <c r="H31" s="5"/>
       <c r="I31" s="3"/>
     </row>
-    <row r="32" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="13">
         <v>3.3</v>
       </c>
@@ -1580,7 +1580,7 @@
       <c r="H32" s="16"/>
       <c r="I32" s="14"/>
     </row>
-    <row r="33" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="2" t="s">
         <v>7</v>
       </c>
@@ -1600,7 +1600,7 @@
       <c r="H33" s="5"/>
       <c r="I33" s="3"/>
     </row>
-    <row r="34" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="2" t="s">
         <v>76</v>
       </c>
@@ -1620,7 +1620,7 @@
       <c r="H34" s="5"/>
       <c r="I34" s="3"/>
     </row>
-    <row r="35" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="14">
         <v>3.4</v>
       </c>
@@ -1640,7 +1640,7 @@
       <c r="H35" s="16"/>
       <c r="I35" s="14"/>
     </row>
-    <row r="36" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="14">
         <v>3.5</v>
       </c>
@@ -1660,7 +1660,7 @@
       <c r="H36" s="16"/>
       <c r="I36" s="14"/>
     </row>
-    <row r="37" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="2" t="s">
         <v>66</v>
       </c>
@@ -1680,7 +1680,7 @@
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
     </row>
-    <row r="38" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="8">
         <v>4</v>
       </c>
@@ -1697,7 +1697,7 @@
       <c r="H38" s="11"/>
       <c r="I38" s="9"/>
     </row>
-    <row r="39" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="14">
         <v>4.0999999999999996</v>
       </c>
@@ -1717,7 +1717,7 @@
       <c r="H39" s="16"/>
       <c r="I39" s="14"/>
     </row>
-    <row r="40" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="14">
         <v>4.2</v>
       </c>
@@ -1737,7 +1737,7 @@
       <c r="H40" s="13"/>
       <c r="I40" s="13"/>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B41" s="8">
         <v>5</v>
       </c>
@@ -1754,7 +1754,7 @@
       <c r="H41" s="11"/>
       <c r="I41" s="9"/>
     </row>
-    <row r="42" spans="2:9" s="6" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:9" s="6" customFormat="1" ht="49.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="14">
         <v>5.0999999999999996</v>
       </c>

</xml_diff>